<commit_message>
Add preliminary statistics tables for Taiwan's customs imports and exports
</commit_message>
<xml_diff>
--- a/data/August2025_PreliminaryStatistics_on_CustomsImports_and_Exports/Table8_Taiwans's_ExportValue_and_AnnualGrowthRate.xlsx
+++ b/data/August2025_PreliminaryStatistics_on_CustomsImports_and_Exports/Table8_Taiwans's_ExportValue_and_AnnualGrowthRate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\貿易統計科\記者會資料檔\news上網檔\114年8月\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AboutCoding\CourseCode\Artificial_Intelligence_Practice_CourseCode\ROC_PreliminaryStatistics_on_CustomsImports_and_Exports_for_2025\data\August2025_PreliminaryStatistics_on_CustomsImports_and_Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65DD2F5-A228-4F4B-B7DA-981E7172DB3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9069146F-CB4C-403F-965B-0F59C8F89895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="表8" sheetId="1" r:id="rId1"/>
@@ -942,7 +942,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1057,6 +1057,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1487,7 +1499,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1521,16 +1533,16 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="35" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="35" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="177" fontId="36" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="36" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1">
@@ -1551,10 +1563,7 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="3" fontId="38" fillId="0" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1566,10 +1575,7 @@
     <xf numFmtId="198" fontId="13" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="198" fontId="35" fillId="0" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="198" fontId="35" fillId="0" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="198" fontId="35" fillId="0" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="198" fontId="35" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1597,10 +1603,10 @@
     <xf numFmtId="199" fontId="13" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="199" fontId="35" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="199" fontId="36" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="199" fontId="35" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="199" fontId="36" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="199" fontId="36" fillId="0" borderId="1" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1610,23 +1616,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="199" fontId="30" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="199" fontId="35" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="199" fontId="35" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="199" fontId="36" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="199" fontId="36" fillId="0" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="199" fontId="36" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="199" fontId="29" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="199" fontId="30" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="199" fontId="13" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="199" fontId="13" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="199" fontId="38" fillId="0" borderId="14" xfId="45" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1662,7 +1658,7 @@
     <xf numFmtId="3" fontId="38" fillId="0" borderId="22" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1">
@@ -1691,6 +1687,60 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="12" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="177" fontId="36" fillId="24" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="199" fontId="36" fillId="24" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="198" fontId="36" fillId="24" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="199" fontId="36" fillId="24" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="18" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="19" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="20" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="38" fillId="25" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="198" fontId="38" fillId="25" borderId="14" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="199" fontId="38" fillId="25" borderId="14" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="35" fillId="25" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="198" fontId="35" fillId="25" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="199" fontId="35" fillId="25" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="198" fontId="35" fillId="25" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="36" fillId="25" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="198" fontId="36" fillId="25" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="199" fontId="36" fillId="25" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="72">
@@ -1781,7 +1831,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="表6"/>
@@ -1850,9 +1900,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1890,9 +1940,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1925,26 +1975,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1977,26 +2010,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2173,8 +2189,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="7" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
       <selection pane="bottomRight" sqref="A1:R1"/>
@@ -2184,67 +2200,67 @@
   <cols>
     <col min="1" max="1" width="15.6640625" style="18" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="43" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" style="41" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" style="34" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" style="43" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" style="32" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" style="41" customWidth="1"/>
     <col min="7" max="7" width="8.109375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" style="34" customWidth="1"/>
-    <col min="9" max="9" width="5.88671875" style="43" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" style="32" customWidth="1"/>
+    <col min="9" max="9" width="5.88671875" style="41" customWidth="1"/>
     <col min="10" max="10" width="8.109375" style="21" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" style="34" customWidth="1"/>
-    <col min="12" max="12" width="5.88671875" style="49" customWidth="1"/>
+    <col min="11" max="11" width="7.109375" style="32" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" style="41" customWidth="1"/>
     <col min="13" max="13" width="8.109375" style="21" customWidth="1"/>
-    <col min="14" max="14" width="5.88671875" style="43" customWidth="1"/>
+    <col min="14" max="14" width="5.88671875" style="41" customWidth="1"/>
     <col min="15" max="15" width="8.109375" style="21" customWidth="1"/>
-    <col min="16" max="16" width="5.88671875" style="43" customWidth="1"/>
+    <col min="16" max="16" width="5.88671875" style="41" customWidth="1"/>
     <col min="17" max="17" width="8.109375" style="21" customWidth="1"/>
-    <col min="18" max="18" width="5.88671875" style="43" customWidth="1"/>
+    <col min="18" max="18" width="5.88671875" style="41" customWidth="1"/>
     <col min="19" max="20" width="8.44140625" style="21" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="10.44140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="1" customFormat="1" ht="26.1" customHeight="1">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
     </row>
     <row r="2" spans="1:28" s="4" customFormat="1" ht="12" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="37"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="37"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="37"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="35"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="48"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="35"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="37"/>
+      <c r="N2" s="35"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="37"/>
+      <c r="P2" s="35"/>
       <c r="Q2" s="3"/>
-      <c r="R2" s="48"/>
+      <c r="R2" s="35"/>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
@@ -2252,98 +2268,98 @@
       <c r="AB2" s="5"/>
     </row>
     <row r="3" spans="1:28" s="6" customFormat="1" ht="15.9" customHeight="1" thickBot="1">
-      <c r="C3" s="38"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="38"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="36"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="38"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="36"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="50"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="44"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="38"/>
+      <c r="N3" s="36"/>
       <c r="O3" s="8"/>
-      <c r="P3" s="38"/>
+      <c r="P3" s="36"/>
       <c r="Q3" s="8"/>
-      <c r="R3" s="50" t="s">
+      <c r="R3" s="44" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:28" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="64" t="s">
+      <c r="C4" s="60"/>
+      <c r="D4" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="65"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="64" t="s">
+      <c r="E4" s="59"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="67" t="s">
+      <c r="H4" s="72"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="68"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="65" t="s">
+      <c r="K4" s="62"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="66"/>
-      <c r="O4" s="64" t="s">
+      <c r="N4" s="60"/>
+      <c r="O4" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="64" t="s">
+      <c r="P4" s="60"/>
+      <c r="Q4" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="65"/>
+      <c r="R4" s="59"/>
     </row>
     <row r="5" spans="1:28" s="9" customFormat="1" ht="24" customHeight="1">
-      <c r="A5" s="71"/>
+      <c r="A5" s="65"/>
       <c r="B5" s="10"/>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="52" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="52" t="s">
+      <c r="G5" s="74"/>
+      <c r="H5" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="51" t="s">
+      <c r="I5" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="61"/>
-      <c r="K5" s="52" t="s">
+      <c r="J5" s="55"/>
+      <c r="K5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="51" t="s">
+      <c r="L5" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="25"/>
-      <c r="N5" s="51" t="s">
+      <c r="M5" s="24"/>
+      <c r="N5" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="25"/>
-      <c r="P5" s="51" t="s">
+      <c r="O5" s="24"/>
+      <c r="P5" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="53" t="s">
+      <c r="Q5" s="24"/>
+      <c r="R5" s="47" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2354,52 +2370,52 @@
       <c r="B6" s="11">
         <v>284433.978</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="37">
         <v>-10.951109063801775</v>
       </c>
       <c r="D6" s="11">
         <v>112386.42600000001</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="27">
         <v>39.512306789169891</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="37">
         <v>-12.526875160743497</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="77">
         <v>34448.478999999999</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="78">
         <v>12.111239044724819</v>
       </c>
-      <c r="I6" s="39">
+      <c r="I6" s="79">
         <v>-1.6692699532921254</v>
       </c>
       <c r="J6" s="11">
         <v>51590.504000000001</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K6" s="27">
         <v>18.137953968354655</v>
       </c>
-      <c r="L6" s="39">
+      <c r="L6" s="37">
         <v>-14.148165838163235</v>
       </c>
       <c r="M6" s="11">
         <v>19556.522000000001</v>
       </c>
-      <c r="N6" s="39">
+      <c r="N6" s="37">
         <v>-2.8447071526215955</v>
       </c>
       <c r="O6" s="11">
         <v>12772.06</v>
       </c>
-      <c r="P6" s="39">
+      <c r="P6" s="37">
         <v>-0.66310874476309911</v>
       </c>
       <c r="Q6" s="11">
         <v>25869.494999999999</v>
       </c>
-      <c r="R6" s="39">
+      <c r="R6" s="37">
         <v>-11.011562358910412</v>
       </c>
     </row>
@@ -2410,52 +2426,52 @@
       <c r="B7" s="11">
         <v>279174.65600000002</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="37">
         <v>-1.8490484283843189</v>
       </c>
       <c r="D7" s="11">
         <v>111986.143</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="27">
         <v>40.113291301055639</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="37">
         <v>-0.35616667799365737</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="77">
         <v>33396.311000000002</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="78">
         <v>11.962515322307766</v>
       </c>
-      <c r="I7" s="39">
+      <c r="I7" s="79">
         <v>-3.0543235305105925</v>
       </c>
       <c r="J7" s="11">
         <v>51248.027999999998</v>
       </c>
-      <c r="K7" s="29">
+      <c r="K7" s="27">
         <v>18.356977217874675</v>
       </c>
-      <c r="L7" s="39">
+      <c r="L7" s="37">
         <v>-0.66383534458201843</v>
       </c>
       <c r="M7" s="11">
         <v>19470.701000000001</v>
       </c>
-      <c r="N7" s="39">
+      <c r="N7" s="37">
         <v>-0.43883569890392582</v>
       </c>
       <c r="O7" s="11">
         <v>12531.227000000001</v>
       </c>
-      <c r="P7" s="39">
+      <c r="P7" s="37">
         <v>-1.8856237756477812</v>
       </c>
       <c r="Q7" s="11">
         <v>26123.541000000001</v>
       </c>
-      <c r="R7" s="39">
+      <c r="R7" s="37">
         <v>0.98202922012973182</v>
       </c>
     </row>
@@ -2466,52 +2482,52 @@
       <c r="B8" s="11">
         <v>315486.658</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="37">
         <v>13.006912060097603</v>
       </c>
       <c r="D8" s="11">
         <v>129910.59299999999</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="27">
         <v>41.177840553878511</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="37">
         <v>16.005953522303201</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="77">
         <v>36772.593000000001</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="78">
         <v>11.65583141712446</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="79">
         <v>10.109745354808799</v>
       </c>
       <c r="J8" s="11">
         <v>58518.29</v>
       </c>
-      <c r="K8" s="29">
+      <c r="K8" s="27">
         <v>18.54857836809061</v>
       </c>
-      <c r="L8" s="39">
+      <c r="L8" s="37">
         <v>14.186422939044602</v>
       </c>
       <c r="M8" s="11">
         <v>20573.772000000001</v>
       </c>
-      <c r="N8" s="39">
+      <c r="N8" s="37">
         <v>5.6652865246094635</v>
       </c>
       <c r="O8" s="11">
         <v>14415.736000000001</v>
       </c>
-      <c r="P8" s="39">
+      <c r="P8" s="37">
         <v>15.038503412315491</v>
       </c>
       <c r="Q8" s="11">
         <v>28778.05</v>
       </c>
-      <c r="R8" s="39">
+      <c r="R8" s="37">
         <v>10.161367480771462</v>
       </c>
     </row>
@@ -2522,52 +2538,52 @@
       <c r="B9" s="11">
         <v>334007.33799999999</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="37">
         <v>5.8705113291985871</v>
       </c>
       <c r="D9" s="11">
         <v>137898.804</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="27">
         <v>41.286160006460698</v>
       </c>
-      <c r="F9" s="39">
+      <c r="F9" s="37">
         <v>6.1490066479798147</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="77">
         <v>39490.379999999997</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="78">
         <v>11.823207309295702</v>
       </c>
-      <c r="I9" s="39">
+      <c r="I9" s="79">
         <v>7.3907950956844406</v>
       </c>
       <c r="J9" s="11">
         <v>58125.724999999999</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="27">
         <v>17.402529342034995</v>
       </c>
-      <c r="L9" s="39">
+      <c r="L9" s="37">
         <v>-0.67084154372931948</v>
       </c>
       <c r="M9" s="11">
         <v>22800.956999999999</v>
       </c>
-      <c r="N9" s="39">
+      <c r="N9" s="37">
         <v>10.825360561009425</v>
       </c>
       <c r="O9" s="11">
         <v>15738.931</v>
       </c>
-      <c r="P9" s="39">
+      <c r="P9" s="37">
         <v>9.178823752044293</v>
       </c>
       <c r="Q9" s="11">
         <v>31277.632000000001</v>
       </c>
-      <c r="R9" s="39">
+      <c r="R9" s="37">
         <v>8.6857240153519779</v>
       </c>
     </row>
@@ -2578,332 +2594,332 @@
       <c r="B10" s="11">
         <v>329157.32</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="37">
         <v>-1.4520692955554169</v>
       </c>
       <c r="D10" s="11">
         <v>132114.565</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <v>40.137210073286539</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="37">
         <v>-4.1945534204923192</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="77">
         <v>46247.108</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="78">
         <v>14.050153282327127</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="79">
         <v>17.109807502485417</v>
       </c>
       <c r="J10" s="11">
         <v>53934.743000000002</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="27">
         <v>16.385703650764931</v>
       </c>
-      <c r="L10" s="39">
+      <c r="L10" s="37">
         <v>-7.2102016792048609</v>
       </c>
       <c r="M10" s="11">
         <v>23278.741000000002</v>
       </c>
-      <c r="N10" s="39">
+      <c r="N10" s="37">
         <v>2.0954559056446622</v>
       </c>
       <c r="O10" s="11">
         <v>16917.052</v>
       </c>
-      <c r="P10" s="39">
+      <c r="P10" s="37">
         <v>7.4853940207247875</v>
       </c>
       <c r="Q10" s="11">
         <v>29770.313999999998</v>
       </c>
-      <c r="R10" s="39">
+      <c r="R10" s="37">
         <v>-4.8191563862635123</v>
       </c>
     </row>
     <row r="11" spans="1:28" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="11">
         <v>345125.94400000002</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="37">
         <v>4.8513652985144002</v>
       </c>
       <c r="D11" s="11">
         <v>151381.35999999999</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="27">
         <v>43.862642792220804</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="37">
         <v>14.583399642575367</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="77">
         <v>50549.921000000002</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="78">
         <v>14.646804124351775</v>
       </c>
-      <c r="I11" s="39">
+      <c r="I11" s="79">
         <v>9.3039612336408144</v>
       </c>
       <c r="J11" s="11">
         <v>53215.33</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="27">
         <v>15.419104511018736</v>
       </c>
-      <c r="L11" s="39">
+      <c r="L11" s="37">
         <v>-1.3338582145464195</v>
       </c>
       <c r="M11" s="11">
         <v>23398.254000000001</v>
       </c>
-      <c r="N11" s="39">
+      <c r="N11" s="37">
         <v>0.51339975817420702</v>
       </c>
       <c r="O11" s="11">
         <v>15140.525</v>
       </c>
-      <c r="P11" s="39">
+      <c r="P11" s="37">
         <v>-10.501398234160419</v>
       </c>
       <c r="Q11" s="11">
         <v>28143.108</v>
       </c>
-      <c r="R11" s="39">
+      <c r="R11" s="37">
         <v>-5.4658677768732975</v>
       </c>
     </row>
     <row r="12" spans="1:28" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="11">
         <v>446371.19099999999</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="37">
         <v>29.335739245381099</v>
       </c>
       <c r="D12" s="11">
         <v>188874.56099999999</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="28">
         <v>42.313340289024168</v>
       </c>
-      <c r="F12" s="39">
+      <c r="F12" s="37">
         <v>24.767382853476807</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="77">
         <v>65685.966</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="80">
         <v>14.715547805144979</v>
       </c>
-      <c r="I12" s="39">
+      <c r="I12" s="79">
         <v>29.942766873958121</v>
       </c>
       <c r="J12" s="11">
         <v>70241.748999999996</v>
       </c>
-      <c r="K12" s="30">
+      <c r="K12" s="28">
         <v>15.736174380483261</v>
       </c>
-      <c r="L12" s="39">
+      <c r="L12" s="37">
         <v>31.995327286328955</v>
       </c>
       <c r="M12" s="11">
         <v>29206.218000000001</v>
       </c>
-      <c r="N12" s="39">
+      <c r="N12" s="37">
         <v>24.822211093186695</v>
       </c>
       <c r="O12" s="11">
         <v>20140.178</v>
       </c>
-      <c r="P12" s="39">
+      <c r="P12" s="37">
         <v>33.021662062577093</v>
       </c>
       <c r="Q12" s="11">
         <v>38484.235999999997</v>
       </c>
-      <c r="R12" s="39">
+      <c r="R12" s="37">
         <v>36.744797340791216</v>
       </c>
     </row>
     <row r="13" spans="1:28" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="11">
         <v>479415.23</v>
       </c>
-      <c r="C13" s="39">
+      <c r="C13" s="37">
         <v>7.4028162359608904</v>
       </c>
       <c r="D13" s="11">
         <v>185875.17800000001</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="28">
         <v>38.771229274464226</v>
       </c>
-      <c r="F13" s="39">
+      <c r="F13" s="37">
         <v>-1.5880291046712216</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="77">
         <v>75052.058999999994</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="80">
         <v>15.654917554454832</v>
       </c>
-      <c r="I13" s="39">
+      <c r="I13" s="79">
         <v>14.258895119240538</v>
       </c>
       <c r="J13" s="11">
         <v>80609.433999999994</v>
       </c>
-      <c r="K13" s="30">
+      <c r="K13" s="28">
         <v>16.814116230725503</v>
       </c>
-      <c r="L13" s="39">
+      <c r="L13" s="37">
         <v>14.760004053999282</v>
       </c>
       <c r="M13" s="11">
         <v>33608.898999999998</v>
       </c>
-      <c r="N13" s="39">
+      <c r="N13" s="37">
         <v>15.074464622567701</v>
       </c>
       <c r="O13" s="11">
         <v>22178.146000000001</v>
       </c>
-      <c r="P13" s="39">
+      <c r="P13" s="37">
         <v>10.118917519001073</v>
       </c>
       <c r="Q13" s="11">
         <v>41099.082999999999</v>
       </c>
-      <c r="R13" s="39">
+      <c r="R13" s="37">
         <v>6.7945924663802604</v>
       </c>
     </row>
     <row r="14" spans="1:28" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="23" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="11">
         <v>432419.962</v>
       </c>
-      <c r="C14" s="39">
+      <c r="C14" s="37">
         <v>-9.8026230831256651</v>
       </c>
       <c r="D14" s="11">
         <v>152238.74100000001</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="28">
         <v>35.206224128940647</v>
       </c>
-      <c r="F14" s="39">
+      <c r="F14" s="37">
         <v>-18.096250054431689</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="77">
         <v>76234.038</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="80">
         <v>17.629629688557255</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="79">
         <v>1.5748788450960418</v>
       </c>
       <c r="J14" s="11">
         <v>76274.869000000006</v>
       </c>
-      <c r="K14" s="30">
+      <c r="K14" s="28">
         <v>17.63907212960719</v>
       </c>
-      <c r="L14" s="39">
+      <c r="L14" s="37">
         <v>-5.3772428175094245</v>
       </c>
       <c r="M14" s="11">
         <v>31434.885999999999</v>
       </c>
-      <c r="N14" s="39">
+      <c r="N14" s="37">
         <v>-6.4685635789497304</v>
       </c>
       <c r="O14" s="11">
         <v>18203.298999999999</v>
       </c>
-      <c r="P14" s="39">
+      <c r="P14" s="37">
         <v>-17.922359244997306</v>
       </c>
       <c r="Q14" s="11">
         <v>42283.483</v>
       </c>
-      <c r="R14" s="39">
+      <c r="R14" s="37">
         <v>2.8818161222721197</v>
       </c>
     </row>
     <row r="15" spans="1:28" s="12" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="23" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="11">
         <v>474995.71100000001</v>
       </c>
-      <c r="C15" s="39">
+      <c r="C15" s="37">
         <v>9.8459258918301273</v>
       </c>
       <c r="D15" s="11">
         <v>150611.402</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="28">
         <v>31.707949885046439</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="42">
         <v>-1.0689388189304587</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="77">
         <v>111361.639</v>
       </c>
-      <c r="H15" s="30">
+      <c r="H15" s="80">
         <v>23.444767272856488</v>
       </c>
-      <c r="I15" s="39">
+      <c r="I15" s="79">
         <v>46.078630912873855</v>
       </c>
       <c r="J15" s="11">
         <v>87767.813999999998</v>
       </c>
-      <c r="K15" s="30">
+      <c r="K15" s="28">
         <v>18.477601369331101</v>
       </c>
-      <c r="L15" s="39">
+      <c r="L15" s="37">
         <v>15.067800378654205</v>
       </c>
       <c r="M15" s="11">
         <v>25835.968000000001</v>
       </c>
-      <c r="N15" s="39">
+      <c r="N15" s="37">
         <v>-17.81116050492437</v>
       </c>
       <c r="O15" s="11">
         <v>20792.356</v>
       </c>
-      <c r="P15" s="39">
+      <c r="P15" s="37">
         <v>14.223009796191338</v>
       </c>
       <c r="Q15" s="11">
         <v>38635.423999999999</v>
       </c>
-      <c r="R15" s="39">
+      <c r="R15" s="37">
         <v>-8.6276218068412192</v>
       </c>
     </row>
@@ -2914,52 +2930,52 @@
       <c r="B16" s="14">
         <v>43625.148000000001</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="38">
         <v>16.785654224724446</v>
       </c>
       <c r="D16" s="14">
         <v>13106.584000000001</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="29">
         <v>30.04364363417174</v>
       </c>
-      <c r="F16" s="40">
+      <c r="F16" s="38">
         <v>1.0105693378992866</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="81">
         <v>11882.597</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="82">
         <v>27.237952293021443</v>
       </c>
-      <c r="I16" s="40">
+      <c r="I16" s="83">
         <v>78.446202419489993</v>
       </c>
       <c r="J16" s="14">
         <v>7253.6819999999998</v>
       </c>
-      <c r="K16" s="31">
+      <c r="K16" s="29">
         <v>16.627294880466653</v>
       </c>
-      <c r="L16" s="40">
+      <c r="L16" s="38">
         <v>5.5757778113184697</v>
       </c>
       <c r="M16" s="14">
         <v>2073.48</v>
       </c>
-      <c r="N16" s="40">
+      <c r="N16" s="38">
         <v>-17.543598720770145</v>
       </c>
       <c r="O16" s="14">
         <v>2037.7280000000001</v>
       </c>
-      <c r="P16" s="40">
+      <c r="P16" s="38">
         <v>34.344590425054982</v>
       </c>
       <c r="Q16" s="14">
         <v>3694.3780000000002</v>
       </c>
-      <c r="R16" s="40">
+      <c r="R16" s="38">
         <v>2.5485737380376863</v>
       </c>
     </row>
@@ -2970,52 +2986,52 @@
       <c r="B17" s="14">
         <v>40554.747000000003</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="38">
         <v>4.5086398556975489</v>
       </c>
       <c r="D17" s="14">
         <v>14055.977000000001</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="29">
         <v>34.659264425937607</v>
       </c>
-      <c r="F17" s="40">
+      <c r="F17" s="38">
         <v>1.6821272317784079</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="81">
         <v>8780.8230000000003</v>
       </c>
-      <c r="H17" s="31">
+      <c r="H17" s="82">
         <v>21.651776054724248</v>
       </c>
-      <c r="I17" s="40">
+      <c r="I17" s="83">
         <v>27.311516871689555</v>
       </c>
       <c r="J17" s="14">
         <v>7287.75</v>
       </c>
-      <c r="K17" s="31">
+      <c r="K17" s="29">
         <v>17.970152791237979</v>
       </c>
-      <c r="L17" s="40">
+      <c r="L17" s="38">
         <v>-2.4136184271047707</v>
       </c>
       <c r="M17" s="14">
         <v>2200.393</v>
       </c>
-      <c r="N17" s="40">
+      <c r="N17" s="38">
         <v>0.38806745055744207</v>
       </c>
       <c r="O17" s="14">
         <v>1932.8030000000001</v>
       </c>
-      <c r="P17" s="40">
+      <c r="P17" s="38">
         <v>34.952203338469907</v>
       </c>
       <c r="Q17" s="14">
         <v>2960.22</v>
       </c>
-      <c r="R17" s="40">
+      <c r="R17" s="38">
         <v>-19.408590133567614</v>
       </c>
     </row>
@@ -3026,52 +3042,52 @@
       <c r="B18" s="14">
         <v>41291.519999999997</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="38">
         <v>8.4048582596302381</v>
       </c>
       <c r="D18" s="14">
         <v>13869.901</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="29">
         <v>33.590192368796309</v>
       </c>
-      <c r="F18" s="40">
+      <c r="F18" s="38">
         <v>-2.1438619669703898</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="81">
         <v>8649.7150000000001</v>
       </c>
-      <c r="H18" s="31">
+      <c r="H18" s="82">
         <v>20.947921025915246</v>
       </c>
-      <c r="I18" s="40">
+      <c r="I18" s="83">
         <v>20.442208740605025</v>
       </c>
       <c r="J18" s="14">
         <v>7677.8590000000004</v>
       </c>
-      <c r="K18" s="31">
+      <c r="K18" s="29">
         <v>18.594275531634583</v>
       </c>
-      <c r="L18" s="40">
+      <c r="L18" s="38">
         <v>13.05173735941159</v>
       </c>
       <c r="M18" s="14">
         <v>2045.627</v>
       </c>
-      <c r="N18" s="40">
+      <c r="N18" s="38">
         <v>-15.72907436267246</v>
       </c>
       <c r="O18" s="14">
         <v>1885.693</v>
       </c>
-      <c r="P18" s="40">
+      <c r="P18" s="38">
         <v>21.447860694787131</v>
       </c>
       <c r="Q18" s="14">
         <v>3226.4490000000001</v>
       </c>
-      <c r="R18" s="40">
+      <c r="R18" s="38">
         <v>2.0807205022710273</v>
       </c>
     </row>
@@ -3082,52 +3098,52 @@
       <c r="B19" s="14">
         <v>41083.046999999999</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="38">
         <v>9.6824477448486377</v>
       </c>
       <c r="D19" s="14">
         <v>13917.069</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="29">
         <v>33.875454758747573</v>
       </c>
-      <c r="F19" s="40">
+      <c r="F19" s="38">
         <v>9.5319474466480063</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="81">
         <v>8649.1209999999992</v>
       </c>
-      <c r="H19" s="31">
+      <c r="H19" s="82">
         <v>21.052773909393817</v>
       </c>
-      <c r="I19" s="40">
+      <c r="I19" s="83">
         <v>10.573399881847028</v>
       </c>
       <c r="J19" s="14">
         <v>7585.4589999999998</v>
       </c>
-      <c r="K19" s="31">
+      <c r="K19" s="29">
         <v>18.463720570677246</v>
       </c>
-      <c r="L19" s="40">
+      <c r="L19" s="38">
         <v>10.469710339295521</v>
       </c>
       <c r="M19" s="14">
         <v>2326.7139999999999</v>
       </c>
-      <c r="N19" s="40">
+      <c r="N19" s="38">
         <v>-11.200256776154013</v>
       </c>
       <c r="O19" s="14">
         <v>2012.002</v>
       </c>
-      <c r="P19" s="40">
+      <c r="P19" s="38">
         <v>40.303059886753509</v>
       </c>
       <c r="Q19" s="14">
         <v>3002.3020000000001</v>
       </c>
-      <c r="R19" s="40">
+      <c r="R19" s="38">
         <v>-1.2340228711361945</v>
       </c>
     </row>
@@ -3138,108 +3154,108 @@
       <c r="B20" s="14">
         <v>43567.561000000002</v>
       </c>
-      <c r="C20" s="40">
+      <c r="C20" s="38">
         <v>9.1360723704098792</v>
       </c>
       <c r="D20" s="14">
         <v>13828.147000000001</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="29">
         <v>31.739548146842555</v>
       </c>
-      <c r="F20" s="40">
+      <c r="F20" s="38">
         <v>3.5702676500494626</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="81">
         <v>9843.6080000000002</v>
       </c>
-      <c r="H20" s="31">
+      <c r="H20" s="82">
         <v>22.593892735928002</v>
       </c>
-      <c r="I20" s="40">
+      <c r="I20" s="83">
         <v>15.95414186807394</v>
       </c>
       <c r="J20" s="14">
         <v>8905.9359999999997</v>
       </c>
-      <c r="K20" s="31">
+      <c r="K20" s="29">
         <v>20.441667597596293</v>
       </c>
-      <c r="L20" s="40">
+      <c r="L20" s="38">
         <v>27.767529713409029</v>
       </c>
       <c r="M20" s="14">
         <v>2274.5410000000002</v>
       </c>
-      <c r="N20" s="40">
+      <c r="N20" s="38">
         <v>-20.065555956967966</v>
       </c>
       <c r="O20" s="14">
         <v>1962.145</v>
       </c>
-      <c r="P20" s="40">
+      <c r="P20" s="38">
         <v>21.061025796062413</v>
       </c>
       <c r="Q20" s="14">
         <v>3085.049</v>
       </c>
-      <c r="R20" s="40">
+      <c r="R20" s="38">
         <v>-15.671464524218306</v>
       </c>
     </row>
     <row r="21" spans="1:18" s="15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A21" s="62" t="s">
+      <c r="A21" s="56" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="11">
         <v>398434.34499999997</v>
       </c>
-      <c r="C21" s="39">
+      <c r="C21" s="37">
         <v>29.15262506857562</v>
       </c>
       <c r="D21" s="11">
         <v>108729.613</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="28">
         <v>27.289216997595929</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F21" s="37">
         <v>14.524183974629617</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="77">
         <v>117173.944</v>
       </c>
-      <c r="H21" s="30">
+      <c r="H21" s="80">
         <v>29.408595285629808</v>
       </c>
-      <c r="I21" s="39">
+      <c r="I21" s="79">
         <v>55.324062401558713</v>
       </c>
       <c r="J21" s="11">
         <v>77828.706999999995</v>
       </c>
-      <c r="K21" s="30">
+      <c r="K21" s="28">
         <v>19.533634079662484</v>
       </c>
-      <c r="L21" s="39">
+      <c r="L21" s="37">
         <v>38.212728603974973</v>
       </c>
       <c r="M21" s="11">
         <v>19250.373</v>
       </c>
-      <c r="N21" s="39">
+      <c r="N21" s="37">
         <v>13.312854614536857</v>
       </c>
       <c r="O21" s="11">
         <v>16354.188</v>
       </c>
-      <c r="P21" s="39">
+      <c r="P21" s="37">
         <v>25.804223524011643</v>
       </c>
       <c r="Q21" s="11">
         <v>24593.634999999998</v>
       </c>
-      <c r="R21" s="39">
+      <c r="R21" s="37">
         <v>-6.7058985173930798</v>
       </c>
     </row>
@@ -3250,52 +3266,52 @@
       <c r="B22" s="14">
         <v>38707.122000000003</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C22" s="38">
         <v>4.3811944874109914</v>
       </c>
       <c r="D22" s="14">
         <v>10712.05</v>
       </c>
-      <c r="E22" s="31">
+      <c r="E22" s="29">
         <v>27.674622773555729</v>
       </c>
-      <c r="F22" s="40">
+      <c r="F22" s="38">
         <v>-11.727221246545577</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="81">
         <v>8454.1489999999994</v>
       </c>
-      <c r="H22" s="31">
+      <c r="H22" s="82">
         <v>21.841326771853513</v>
       </c>
-      <c r="I22" s="40">
+      <c r="I22" s="83">
         <v>0.68596014173436903</v>
       </c>
       <c r="J22" s="14">
         <v>8284.4060000000009</v>
       </c>
-      <c r="K22" s="31">
+      <c r="K22" s="29">
         <v>21.402795072183356</v>
       </c>
-      <c r="L22" s="40">
+      <c r="L22" s="38">
         <v>21.517967246616138</v>
       </c>
       <c r="M22" s="14">
         <v>2157.9409999999998</v>
       </c>
-      <c r="N22" s="40">
+      <c r="N22" s="38">
         <v>7.1067095899358623</v>
       </c>
       <c r="O22" s="14">
         <v>1385.375</v>
       </c>
-      <c r="P22" s="40">
+      <c r="P22" s="38">
         <v>-3.1202906303868199</v>
       </c>
       <c r="Q22" s="14">
         <v>2597.395</v>
       </c>
-      <c r="R22" s="40">
+      <c r="R22" s="38">
         <v>-18.301206611783407</v>
       </c>
     </row>
@@ -3306,52 +3322,52 @@
       <c r="B23" s="14">
         <v>41296.519</v>
       </c>
-      <c r="C23" s="40">
+      <c r="C23" s="38">
         <v>31.443122694896452</v>
       </c>
       <c r="D23" s="14">
         <v>11718.044</v>
       </c>
-      <c r="E23" s="31">
+      <c r="E23" s="29">
         <v>28.375379532594501</v>
       </c>
-      <c r="F23" s="40">
+      <c r="F23" s="38">
         <v>27.891702612198412</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="81">
         <v>11772.477999999999</v>
       </c>
-      <c r="H23" s="31">
+      <c r="H23" s="82">
         <v>28.507192095295004</v>
       </c>
-      <c r="I23" s="40">
+      <c r="I23" s="83">
         <v>65.629759358397862</v>
       </c>
       <c r="J23" s="14">
         <v>7689.8990000000003</v>
       </c>
-      <c r="K23" s="31">
+      <c r="K23" s="29">
         <v>18.62117966892076</v>
       </c>
-      <c r="L23" s="40">
+      <c r="L23" s="38">
         <v>17.144336971862899</v>
       </c>
       <c r="M23" s="14">
         <v>2110.5079999999998</v>
       </c>
-      <c r="N23" s="40">
+      <c r="N23" s="38">
         <v>19.129782953752645</v>
       </c>
       <c r="O23" s="14">
         <v>1870.202</v>
       </c>
-      <c r="P23" s="40">
+      <c r="P23" s="38">
         <v>30.651517384904604</v>
       </c>
       <c r="Q23" s="14">
         <v>2623.8539999999998</v>
       </c>
-      <c r="R23" s="40">
+      <c r="R23" s="38">
         <v>-4.9484269429691432</v>
       </c>
     </row>
@@ -3362,108 +3378,108 @@
       <c r="B24" s="14">
         <v>49547.224000000002</v>
       </c>
-      <c r="C24" s="40">
+      <c r="C24" s="38">
         <v>18.545704609231489</v>
       </c>
       <c r="D24" s="14">
         <v>14307.758</v>
       </c>
-      <c r="E24" s="31">
+      <c r="E24" s="29">
         <v>28.87701236299333</v>
       </c>
-      <c r="F24" s="40">
+      <c r="F24" s="38">
         <v>12.588501268097838</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="81">
         <v>12744.688</v>
       </c>
-      <c r="H24" s="31">
+      <c r="H24" s="82">
         <v>25.722304845978861</v>
       </c>
-      <c r="I24" s="40">
+      <c r="I24" s="83">
         <v>39.786996474802628</v>
       </c>
       <c r="J24" s="14">
         <v>10303.474</v>
       </c>
-      <c r="K24" s="31">
+      <c r="K24" s="29">
         <v>20.795259891855899</v>
       </c>
-      <c r="L24" s="40">
+      <c r="L24" s="38">
         <v>15.747118728073739</v>
       </c>
       <c r="M24" s="14">
         <v>2551.9679999999998</v>
       </c>
-      <c r="N24" s="40">
+      <c r="N24" s="38">
         <v>-4.044831779306362</v>
       </c>
       <c r="O24" s="14">
         <v>2265.009</v>
       </c>
-      <c r="P24" s="40">
+      <c r="P24" s="38">
         <v>44.409187065578728</v>
       </c>
       <c r="Q24" s="14">
         <v>3420.1979999999999</v>
       </c>
-      <c r="R24" s="40">
+      <c r="R24" s="38">
         <v>-0.11273173526850304</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="67">
         <v>48643.540999999997</v>
       </c>
-      <c r="C25" s="40">
+      <c r="C25" s="68">
         <v>29.89315196755642</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="67">
         <v>13818.541999999999</v>
       </c>
-      <c r="E25" s="31">
+      <c r="E25" s="69">
         <v>28.407763324631318</v>
       </c>
-      <c r="F25" s="45">
+      <c r="F25" s="70">
         <v>22.252269491894445</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="81">
         <v>13143.804</v>
       </c>
-      <c r="H25" s="31">
+      <c r="H25" s="82">
         <v>27.020656247044183</v>
       </c>
-      <c r="I25" s="40">
+      <c r="I25" s="83">
         <v>29.452382844782171</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="67">
         <v>10458.808000000001</v>
       </c>
-      <c r="K25" s="31">
+      <c r="K25" s="69">
         <v>21.500918282244296</v>
       </c>
-      <c r="L25" s="40">
+      <c r="L25" s="68">
         <v>60.092870570367531</v>
       </c>
-      <c r="M25" s="14">
+      <c r="M25" s="67">
         <v>2176.9859999999999</v>
       </c>
-      <c r="N25" s="40">
+      <c r="N25" s="68">
         <v>12.827074940567165</v>
       </c>
-      <c r="O25" s="14">
+      <c r="O25" s="67">
         <v>1856.192</v>
       </c>
-      <c r="P25" s="40">
+      <c r="P25" s="68">
         <v>33.806991845538114</v>
       </c>
-      <c r="Q25" s="14">
+      <c r="Q25" s="67">
         <v>2699.3049999999998</v>
       </c>
-      <c r="R25" s="40">
+      <c r="R25" s="68">
         <v>-17.410116010530167</v>
       </c>
     </row>
@@ -3474,52 +3490,52 @@
       <c r="B26" s="14">
         <v>51738.875999999997</v>
       </c>
-      <c r="C26" s="40">
+      <c r="C26" s="38">
         <v>38.616027940282898</v>
       </c>
       <c r="D26" s="14">
         <v>14055.683000000001</v>
       </c>
-      <c r="E26" s="31">
+      <c r="E26" s="29">
         <v>27.16657973010469</v>
       </c>
-      <c r="F26" s="40">
+      <c r="F26" s="38">
         <v>16.557539392958358</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="81">
         <v>15511.289000000001</v>
       </c>
-      <c r="H26" s="31">
+      <c r="H26" s="82">
         <v>29.979949699719029</v>
       </c>
-      <c r="I26" s="40">
+      <c r="I26" s="83">
         <v>87.312193167428703</v>
       </c>
       <c r="J26" s="14">
         <v>9831.7440000000006</v>
       </c>
-      <c r="K26" s="31">
+      <c r="K26" s="29">
         <v>19.002623868365443</v>
       </c>
-      <c r="L26" s="40">
+      <c r="L26" s="38">
         <v>52.333567138600046</v>
       </c>
       <c r="M26" s="14">
         <v>2332.5520000000001</v>
       </c>
-      <c r="N26" s="40">
+      <c r="N26" s="38">
         <v>17.467847513262367</v>
       </c>
       <c r="O26" s="14">
         <v>2084.596</v>
       </c>
-      <c r="P26" s="40">
+      <c r="P26" s="38">
         <v>16.635110335258048</v>
       </c>
       <c r="Q26" s="14">
         <v>3319.53</v>
       </c>
-      <c r="R26" s="40">
+      <c r="R26" s="38">
         <v>-0.62899972519429481</v>
       </c>
     </row>
@@ -3530,52 +3546,52 @@
       <c r="B27" s="14">
         <v>53329.266000000003</v>
       </c>
-      <c r="C27" s="40">
+      <c r="C27" s="38">
         <v>33.725012004197914</v>
       </c>
       <c r="D27" s="14">
         <v>14553.287</v>
       </c>
-      <c r="E27" s="31">
+      <c r="E27" s="29">
         <v>27.289494290058297</v>
       </c>
-      <c r="F27" s="40">
+      <c r="F27" s="38">
         <v>13.126970529889867</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="81">
         <v>17272.837</v>
       </c>
-      <c r="H27" s="31">
+      <c r="H27" s="82">
         <v>32.389039444120613</v>
       </c>
-      <c r="I27" s="40">
+      <c r="I27" s="83">
         <v>90.885261547214071</v>
       </c>
       <c r="J27" s="14">
         <v>8992.3870000000006</v>
       </c>
-      <c r="K27" s="31">
+      <c r="K27" s="29">
         <v>16.862011564156912</v>
       </c>
-      <c r="L27" s="40">
+      <c r="L27" s="38">
         <v>28.28430127081873</v>
       </c>
       <c r="M27" s="14">
         <v>2821.03</v>
       </c>
-      <c r="N27" s="40">
+      <c r="N27" s="38">
         <v>25.292130529827737</v>
       </c>
       <c r="O27" s="14">
         <v>2241.6379999999999</v>
       </c>
-      <c r="P27" s="40">
+      <c r="P27" s="38">
         <v>32.613288198883431</v>
       </c>
       <c r="Q27" s="14">
         <v>3416.8429999999998</v>
       </c>
-      <c r="R27" s="40">
+      <c r="R27" s="38">
         <v>-5.4207186030521415</v>
       </c>
     </row>
@@ -3586,52 +3602,52 @@
       <c r="B28" s="14">
         <v>56684.35</v>
       </c>
-      <c r="C28" s="40">
+      <c r="C28" s="38">
         <v>41.982256335202699</v>
       </c>
       <c r="D28" s="14">
         <v>14371.401</v>
       </c>
-      <c r="E28" s="31">
+      <c r="E28" s="29">
         <v>25.353384135127243</v>
       </c>
-      <c r="F28" s="40">
+      <c r="F28" s="38">
         <v>23.878540872011293</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="81">
         <v>18644.548999999999</v>
       </c>
-      <c r="H28" s="31">
+      <c r="H28" s="82">
         <v>32.891881092400283</v>
       </c>
-      <c r="I28" s="40">
+      <c r="I28" s="83">
         <v>62.818576944314351</v>
       </c>
       <c r="J28" s="14">
         <v>11626.159</v>
       </c>
-      <c r="K28" s="31">
+      <c r="K28" s="29">
         <v>20.510350740548315</v>
       </c>
-      <c r="L28" s="40">
+      <c r="L28" s="38">
         <v>71.559913669328026</v>
       </c>
       <c r="M28" s="14">
         <v>2314.1329999999998</v>
       </c>
-      <c r="N28" s="40">
+      <c r="N28" s="38">
         <v>0.50243988875010637</v>
       </c>
       <c r="O28" s="14">
         <v>2096.8629999999998</v>
       </c>
-      <c r="P28" s="40">
+      <c r="P28" s="38">
         <v>25.769420859054669</v>
       </c>
       <c r="Q28" s="14">
         <v>3209.4430000000002</v>
       </c>
-      <c r="R28" s="40">
+      <c r="R28" s="38">
         <v>4.1438602867211385</v>
       </c>
     </row>
@@ -3642,226 +3658,226 @@
       <c r="B29" s="14">
         <v>58487.447</v>
       </c>
-      <c r="C29" s="40">
+      <c r="C29" s="38">
         <v>34.068191585275535</v>
       </c>
       <c r="D29" s="14">
         <v>15192.848</v>
       </c>
-      <c r="E29" s="31">
+      <c r="E29" s="29">
         <v>25.976254357623098</v>
       </c>
-      <c r="F29" s="40">
+      <c r="F29" s="38">
         <v>15.917679236634047</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="81">
         <v>19630.150000000001</v>
       </c>
-      <c r="H29" s="31">
+      <c r="H29" s="82">
         <v>33.563013957507835</v>
       </c>
-      <c r="I29" s="40">
+      <c r="I29" s="83">
         <v>65.200839513449793</v>
       </c>
       <c r="J29" s="14">
         <v>10641.83</v>
       </c>
-      <c r="K29" s="31">
+      <c r="K29" s="29">
         <v>18.195066712349401</v>
       </c>
-      <c r="L29" s="40">
+      <c r="L29" s="38">
         <v>46.709353952930385</v>
       </c>
       <c r="M29" s="14">
         <v>2785.2550000000001</v>
       </c>
-      <c r="N29" s="40">
+      <c r="N29" s="38">
         <v>34.327555606998864</v>
       </c>
       <c r="O29" s="14">
         <v>2554.3130000000001</v>
       </c>
-      <c r="P29" s="40">
+      <c r="P29" s="38">
         <v>25.351028203960489</v>
       </c>
       <c r="Q29" s="14">
         <v>3307.067</v>
       </c>
-      <c r="R29" s="40">
+      <c r="R29" s="38">
         <v>-10.483794565688729</v>
       </c>
     </row>
     <row r="30" spans="1:18" s="12" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="48" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="16">
         <v>1803.097</v>
       </c>
-      <c r="C30" s="41">
+      <c r="C30" s="39">
         <v>3.1809432409474572</v>
       </c>
       <c r="D30" s="16">
         <v>821.447</v>
       </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="46">
+      <c r="E30" s="30"/>
+      <c r="F30" s="43">
         <v>5.7158449618099167</v>
       </c>
       <c r="G30" s="16">
         <v>985.601</v>
       </c>
-      <c r="H30" s="35"/>
-      <c r="I30" s="41">
+      <c r="H30" s="33"/>
+      <c r="I30" s="39">
         <v>5.286268925035408</v>
       </c>
       <c r="J30" s="16">
         <v>-984.32899999999995</v>
       </c>
-      <c r="K30" s="35"/>
-      <c r="L30" s="41">
+      <c r="K30" s="33"/>
+      <c r="L30" s="39">
         <v>-8.4665021354000061</v>
       </c>
       <c r="M30" s="16">
         <v>471.12200000000001</v>
       </c>
-      <c r="N30" s="41">
+      <c r="N30" s="39">
         <v>20.35846686426407</v>
       </c>
       <c r="O30" s="16">
         <v>457.45</v>
       </c>
-      <c r="P30" s="41">
+      <c r="P30" s="39">
         <v>21.815922165635047</v>
       </c>
       <c r="Q30" s="16">
         <v>97.623999999999995</v>
       </c>
-      <c r="R30" s="41">
+      <c r="R30" s="39">
         <v>3.0417739152868584</v>
       </c>
     </row>
     <row r="31" spans="1:18" s="12" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A31" s="55" t="s">
+      <c r="A31" s="49" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="14">
         <v>14862.299000000001</v>
       </c>
-      <c r="C31" s="40">
+      <c r="C31" s="38">
         <v>34.068191585275535</v>
       </c>
       <c r="D31" s="14">
         <v>2086.2640000000001</v>
       </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="40">
+      <c r="E31" s="29"/>
+      <c r="F31" s="38">
         <v>15.917679236634047</v>
       </c>
       <c r="G31" s="14">
         <v>7747.5529999999999</v>
       </c>
-      <c r="H31" s="31"/>
-      <c r="I31" s="40">
+      <c r="H31" s="29"/>
+      <c r="I31" s="38">
         <v>65.200839513449793</v>
       </c>
       <c r="J31" s="14">
         <v>3388.1480000000001</v>
       </c>
-      <c r="K31" s="31"/>
-      <c r="L31" s="40">
+      <c r="K31" s="29"/>
+      <c r="L31" s="38">
         <v>46.709353952930385</v>
       </c>
       <c r="M31" s="14">
         <v>711.77499999999998</v>
       </c>
-      <c r="N31" s="40">
+      <c r="N31" s="38">
         <v>34.327555606998864</v>
       </c>
       <c r="O31" s="14">
         <v>516.58500000000004</v>
       </c>
-      <c r="P31" s="40">
+      <c r="P31" s="38">
         <v>25.351028203960489</v>
       </c>
       <c r="Q31" s="14">
         <v>-387.31099999999998</v>
       </c>
-      <c r="R31" s="40">
+      <c r="R31" s="38">
         <v>-10.483794565688729</v>
       </c>
     </row>
     <row r="32" spans="1:18" s="12" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A32" s="56" t="s">
+      <c r="A32" s="50" t="s">
         <v>13</v>
       </c>
       <c r="B32" s="17">
         <v>89935.509000000005</v>
       </c>
-      <c r="C32" s="42">
+      <c r="C32" s="40">
         <v>29.15262506857562</v>
       </c>
       <c r="D32" s="17">
         <v>13789.305</v>
       </c>
-      <c r="E32" s="33"/>
-      <c r="F32" s="42">
+      <c r="E32" s="31"/>
+      <c r="F32" s="40">
         <v>14.524183974629617</v>
       </c>
       <c r="G32" s="17">
         <v>41735.572</v>
       </c>
-      <c r="H32" s="33"/>
-      <c r="I32" s="42">
+      <c r="H32" s="31"/>
+      <c r="I32" s="40">
         <v>55.324062401558713</v>
       </c>
       <c r="J32" s="17">
         <v>21517.897000000001</v>
       </c>
-      <c r="K32" s="33"/>
-      <c r="L32" s="42">
+      <c r="K32" s="31"/>
+      <c r="L32" s="40">
         <v>38.212728603974973</v>
       </c>
       <c r="M32" s="17">
         <v>2261.6799999999998</v>
       </c>
-      <c r="N32" s="42">
+      <c r="N32" s="40">
         <v>13.312854614536857</v>
       </c>
       <c r="O32" s="17">
         <v>3354.4749999999999</v>
       </c>
-      <c r="P32" s="42">
+      <c r="P32" s="40">
         <v>25.804223524011643</v>
       </c>
       <c r="Q32" s="17">
         <v>-1767.769</v>
       </c>
-      <c r="R32" s="42">
+      <c r="R32" s="40">
         <v>-6.7058985173930798</v>
       </c>
     </row>
     <row r="33" spans="1:31" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A33" s="57" t="s">
+      <c r="A33" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="58"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="59"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="53"/>
       <c r="J33" s="19"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="40"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="47"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="47"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="52"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="52"/>
+      <c r="P33" s="38"/>
       <c r="Q33" s="19"/>
-      <c r="R33" s="47"/>
+      <c r="R33" s="38"/>
       <c r="S33" s="12"/>
       <c r="T33" s="12"/>
       <c r="U33" s="12"/>

</xml_diff>